<commit_message>
Completed initiative workstream controller
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/initiatives/tests_unit/input_data/workstream_controller_INPUT.xlsx
+++ b/src/apodeixi/controllers/initiatives/tests_unit/input_data/workstream_controller_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\initiatives\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882EF898-DD44-47D3-BDC5-EBC040A4D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643D63BB-EACE-4DBC-BE87-8AD753B35EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="2" xr2:uid="{1C3C717C-D18E-4132-9B42-D7001AA1AE8F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="125">
   <si>
     <t>Posting Label</t>
   </si>
@@ -260,9 +260,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Aggregation across all products of the product-specific metrics M5, M6, M7</t>
-  </si>
-  <si>
     <t>Quarterly</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
   </si>
   <si>
     <t>Aggregated # of epics delivered</t>
-  </si>
-  <si>
-    <t>Aggregation across all products of the product-specific metric M8</t>
   </si>
   <si>
     <t>M4</t>
@@ -419,6 +413,12 @@
   </si>
   <si>
     <t>M9</t>
+  </si>
+  <si>
+    <t>Aggregation across all products of the product-specific metric M9</t>
+  </si>
+  <si>
+    <t>Aggregation across all products of the product-specific metrics M6, M7, M8</t>
   </si>
 </sst>
 </file>
@@ -982,10 +982,10 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -1025,28 +1025,28 @@
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>18</v>
@@ -1054,23 +1054,23 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>53</v>
@@ -1078,10 +1078,10 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
@@ -1097,7 +1097,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
@@ -1113,7 +1113,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
@@ -1129,7 +1129,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1143,7 +1143,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1176,7 +1176,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>20</v>
@@ -1566,7 +1566,7 @@
   <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1622,16 +1622,16 @@
         <v>58</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>59</v>
@@ -1717,7 +1717,7 @@
         <v>66</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>68</v>
@@ -1744,16 +1744,16 @@
         <v>69</v>
       </c>
       <c r="O5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="P5" s="14"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B6" s="19" t="s">
+      <c r="C6" s="19" t="s">
         <v>76</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>77</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>73</v>
@@ -1762,17 +1762,33 @@
         <v>66</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="17">
+        <v>1</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1</v>
+      </c>
+      <c r="M6" s="17">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="P6" s="14"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.45">
@@ -1828,19 +1844,19 @@
     </row>
     <row r="10" spans="2:16" ht="114" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>68</v>
@@ -1866,19 +1882,19 @@
     </row>
     <row r="11" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>68</v>
@@ -1904,19 +1920,19 @@
     </row>
     <row r="12" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>68</v>
@@ -1943,24 +1959,24 @@
         <v>69</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>68</v>
@@ -1987,24 +2003,24 @@
         <v>69</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>73</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>68</v>
@@ -2031,27 +2047,27 @@
         <v>69</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="H15" s="17">
         <v>1</v>
@@ -2072,10 +2088,10 @@
         <v>1</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.45">
@@ -2133,29 +2149,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="66517581-92a9-4cb0-981f-3f6c827c3504">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCBD749F692D2840A5441473A3346AC8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2155aeb54e5d7003d408112aa42e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1457f3fe-6304-4719-bef8-60c608407d99" xmlns:ns3="66517581-92a9-4cb0-981f-3f6c827c3504" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4c58ad8abd1e926bea19a7235ad73cd" ns2:_="" ns3:_="">
     <xsd:import namespace="1457f3fe-6304-4719-bef8-60c608407d99"/>
@@ -2366,25 +2359,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6CD186-1AFD-40DE-A756-562BEC0234AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66517581-92a9-4cb0-981f-3f6c827c3504"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F59924-779F-45B5-BAB0-46EB91D29C8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="66517581-92a9-4cb0-981f-3f6c827c3504">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821A1CA1-1BFA-4232-A3C4-563FBA90B62E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2401,4 +2399,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F59924-779F-45B5-BAB0-46EB91D29C8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6CD186-1AFD-40DE-A756-562BEC0234AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="66517581-92a9-4cb0-981f-3f6c827c3504"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Made a more precise distinction between posting API vs manifest API
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/initiatives/tests_unit/input_data/workstream_controller_INPUT.xlsx
+++ b/src/apodeixi/controllers/initiatives/tests_unit/input_data/workstream_controller_INPUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\initiatives\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643D63BB-EACE-4DBC-BE87-8AD753B35EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F5E4D-88C5-4F22-BDF3-2B9B87083554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="2" xr2:uid="{1C3C717C-D18E-4132-9B42-D7001AA1AE8F}"/>
+    <workbookView xWindow="7327" yWindow="3885" windowWidth="12578" windowHeight="11715" xr2:uid="{1C3C717C-D18E-4132-9B42-D7001AA1AE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Posting Label" sheetId="3" r:id="rId1"/>
@@ -337,9 +337,6 @@
     <t>Aha and the the ea-journeys knowledge base system.</t>
   </si>
   <si>
-    <t>excelAPI</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -364,9 +361,6 @@
     <t>Dec 2020</t>
   </si>
   <si>
-    <t>workstream.initiatives.a6i.xlsx/v1a</t>
-  </si>
-  <si>
     <t>joe.theworkstreamlead@mycorp.com</t>
   </si>
   <si>
@@ -419,6 +413,12 @@
   </si>
   <si>
     <t>Aggregation across all products of the product-specific metrics M6, M7, M8</t>
+  </si>
+  <si>
+    <t>manifestAPI</t>
+  </si>
+  <si>
+    <t>workstream.initiatives.a6i.io/v1a</t>
   </si>
 </sst>
 </file>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97241D7-8658-4BD0-A90F-924E588AE6D5}">
   <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -982,10 +982,10 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -1025,28 +1025,28 @@
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>18</v>
@@ -1054,23 +1054,23 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>53</v>
@@ -1078,10 +1078,10 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
@@ -1097,7 +1097,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
@@ -1113,7 +1113,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
@@ -1129,7 +1129,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1176,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>20</v>
@@ -1565,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162FD3B0-E141-42CC-BCBA-81C0D748581F}">
   <dimension ref="B1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1622,16 +1622,16 @@
         <v>58</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>59</v>
@@ -1717,7 +1717,7 @@
         <v>66</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>68</v>
@@ -1762,7 +1762,7 @@
         <v>66</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="17">
@@ -1847,7 +1847,7 @@
         <v>77</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>65</v>
@@ -1885,7 +1885,7 @@
         <v>82</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>65</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="15" spans="2:16" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Renamed posting label field 'environment' to 'knowledgeBase' to avoid confusion with KnowledgeBase environment code
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/initiatives/tests_unit/input_data/workstream_controller_INPUT.xlsx
+++ b/src/apodeixi/controllers/initiatives/tests_unit/input_data/workstream_controller_INPUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\initiatives\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F5E4D-88C5-4F22-BDF3-2B9B87083554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F417705D-3EFC-4B61-BD07-DF120FF6B95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7327" yWindow="3885" windowWidth="12578" windowHeight="11715" xr2:uid="{1C3C717C-D18E-4132-9B42-D7001AA1AE8F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{1C3C717C-D18E-4132-9B42-D7001AA1AE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Posting Label" sheetId="3" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>scenario</t>
   </si>
   <si>
-    <t>environment</t>
-  </si>
-  <si>
     <t>Production</t>
   </si>
   <si>
@@ -419,6 +416,9 @@
   </si>
   <si>
     <t>workstream.initiatives.a6i.io/v1a</t>
+  </si>
+  <si>
+    <t>knowledgeBase</t>
   </si>
 </sst>
 </file>
@@ -965,7 +965,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -982,10 +982,10 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -1025,100 +1025,100 @@
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="10">
         <v>44315</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1162,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1173,44 +1173,44 @@
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>27</v>
       </c>
       <c r="E3" s="15">
         <v>44408</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="15">
         <v>44362</v>
@@ -1224,7 +1224,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="15"/>
       <c r="F4" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="15">
         <v>44392</v>
@@ -1238,7 +1238,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="15"/>
       <c r="F5" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="15">
         <v>44408</v>
@@ -1269,10 +1269,10 @@
     <row r="8" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="E8" s="15">
         <v>44469</v>
@@ -1280,10 +1280,10 @@
       <c r="F8" s="12"/>
       <c r="G8" s="15"/>
       <c r="H8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.45">
@@ -1299,10 +1299,10 @@
     <row r="10" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="15">
         <v>44530</v>
@@ -1310,17 +1310,17 @@
       <c r="F10" s="12"/>
       <c r="G10" s="15"/>
       <c r="H10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="15">
         <v>44712</v>
@@ -1334,7 +1334,7 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="15">
         <v>45077</v>
@@ -1348,7 +1348,7 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="15">
         <v>45443</v>
@@ -1371,16 +1371,16 @@
     <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="8"/>
       <c r="C15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="E15" s="15">
         <v>44804</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="15">
         <v>44408</v>
@@ -1394,7 +1394,7 @@
       <c r="D16" s="12"/>
       <c r="E16" s="15"/>
       <c r="F16" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="15">
         <v>44439</v>
@@ -1406,7 +1406,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="15">
         <v>44712</v>
@@ -1414,17 +1414,17 @@
       <c r="F17" s="12"/>
       <c r="G17" s="15"/>
       <c r="H17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="15">
         <v>45077</v>
@@ -1432,17 +1432,17 @@
       <c r="F18" s="12"/>
       <c r="G18" s="15"/>
       <c r="H18" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="15">
         <v>45443</v>
@@ -1450,10 +1450,10 @@
       <c r="F19" s="12"/>
       <c r="G19" s="15"/>
       <c r="H19" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.45">
@@ -1587,7 +1587,7 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B1" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -1604,46 +1604,46 @@
     </row>
     <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="P2" s="14"/>
     </row>
@@ -1666,103 +1666,103 @@
     </row>
     <row r="4" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>67</v>
-      </c>
       <c r="G4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="P4" s="14"/>
     </row>
     <row r="5" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="P5" s="14"/>
     </row>
     <row r="6" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B6" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>76</v>
-      </c>
       <c r="D6" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="17">
@@ -1784,10 +1784,10 @@
         <v>1</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P6" s="14"/>
     </row>
@@ -1844,230 +1844,230 @@
     </row>
     <row r="10" spans="2:16" ht="114" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>79</v>
-      </c>
       <c r="G10" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N10" s="12" t="s">
+      <c r="O10" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="22" t="s">
-        <v>81</v>
-      </c>
       <c r="G11" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M11" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N11" s="12" t="s">
+      <c r="O11" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="G12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="G13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="G14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O14" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="H15" s="17">
         <v>1</v>
@@ -2088,10 +2088,10 @@
         <v>1</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.45">
@@ -2149,6 +2149,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="66517581-92a9-4cb0-981f-3f6c827c3504">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCBD749F692D2840A5441473A3346AC8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2155aeb54e5d7003d408112aa42e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1457f3fe-6304-4719-bef8-60c608407d99" xmlns:ns3="66517581-92a9-4cb0-981f-3f6c827c3504" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4c58ad8abd1e926bea19a7235ad73cd" ns2:_="" ns3:_="">
     <xsd:import namespace="1457f3fe-6304-4719-bef8-60c608407d99"/>
@@ -2359,30 +2382,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6CD186-1AFD-40DE-A756-562BEC0234AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="66517581-92a9-4cb0-981f-3f6c827c3504"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="66517581-92a9-4cb0-981f-3f6c827c3504">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F59924-779F-45B5-BAB0-46EB91D29C8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821A1CA1-1BFA-4232-A3C4-563FBA90B62E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2399,22 +2417,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F59924-779F-45B5-BAB0-46EB91D29C8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6CD186-1AFD-40DE-A756-562BEC0234AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66517581-92a9-4cb0-981f-3f6c827c3504"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>